<commit_message>
Documentation, mise en page
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/Tests_End-to-end.xlsx
+++ b/2.Documentation/Annexes/Tests_End-to-end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D074E2-E914-E44B-8EA4-771C0F70D001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF317E-D19D-6543-99BE-3B48C76EBE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -93,6 +93,9 @@
     <t>Obtention d'un lien de réinitialisation</t>
   </si>
   <si>
+    <t>KO</t>
+  </si>
+  <si>
     <t>Réinitialisation du mot de passe</t>
   </si>
   <si>
@@ -148,13 +151,43 @@
   </si>
   <si>
     <t>Affichage de la liste des projets en proposition</t>
+  </si>
+  <si>
+    <t>Navigation dans la liste</t>
+  </si>
+  <si>
+    <t>Affichage des projets suivants / précédents</t>
+  </si>
+  <si>
+    <t>Création d'un projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout du projet en haut de liste et message significatif </t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Équipes</t>
+  </si>
+  <si>
+    <t>Affichage de toutes les équipes triées par leur note</t>
+  </si>
+  <si>
+    <t>Rejoindre</t>
+  </si>
+  <si>
+    <t>Quitter</t>
+  </si>
+  <si>
+    <t>Envoie de la requête de demande d'ajout + notification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,8 +217,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +241,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -255,11 +300,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -289,8 +335,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -607,8 +655,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,10 +786,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>1</v>
@@ -752,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>12</v>
@@ -766,10 +814,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>1</v>
@@ -780,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>12</v>
@@ -791,13 +839,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>1</v>
@@ -805,13 +853,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>1</v>
@@ -819,10 +867,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>12</v>
@@ -833,13 +881,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>1</v>
@@ -847,13 +895,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>1</v>
@@ -861,64 +909,95 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="D19" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="18" t="s">
-        <v>1</v>
+      <c r="A20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="18" t="s">
-        <v>1</v>
+      <c r="D21" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D22" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D23" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="18" t="s">
-        <v>1</v>
+      <c r="A24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tests & bugs fixes
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/Tests_End-to-end.xlsx
+++ b/2.Documentation/Annexes/Tests_End-to-end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF317E-D19D-6543-99BE-3B48C76EBE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4648DDF4-CCF1-324F-A4F9-2D1F2BB69D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$D$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$D$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Obtention d'un lien de réinitialisation</t>
   </si>
   <si>
-    <t>KO</t>
-  </si>
-  <si>
     <t>Réinitialisation du mot de passe</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t xml:space="preserve">Ajout du projet en haut de liste et message significatif </t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Équipes</t>
   </si>
   <si>
@@ -181,13 +175,151 @@
   </si>
   <si>
     <t>Envoie de la requête de demande d'ajout + notification</t>
+  </si>
+  <si>
+    <t>Redirection sur la page de login + Message significatif</t>
+  </si>
+  <si>
+    <t>Lecture et suppression d'une notification</t>
+  </si>
+  <si>
+    <t>La notification disparait de la liste</t>
+  </si>
+  <si>
+    <t>Création d'une équipe</t>
+  </si>
+  <si>
+    <t>Ajout de l'équipe en haut de liste + dans la sidebar</t>
+  </si>
+  <si>
+    <t>Acceptation de la requête de "join"</t>
+  </si>
+  <si>
+    <t>Ajout du nouveau membre dans l'équipe + notification</t>
+  </si>
+  <si>
+    <t>Sortie du membre de l'équipe + notification membres de celle-ci</t>
+  </si>
+  <si>
+    <t>Équipe</t>
+  </si>
+  <si>
+    <t>Bannir un utilisateur</t>
+  </si>
+  <si>
+    <t>Sortie le membre de l'équipe + notification a celui-ci</t>
+  </si>
+  <si>
+    <t>Transmetre le leadership de l'équipe à un membre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification du propriétaire + notification </t>
+  </si>
+  <si>
+    <t>Impossible (interdiction + Message d'erreur)</t>
+  </si>
+  <si>
+    <t>Rejoindre une équipe de laquelle ont fait déjà partie</t>
+  </si>
+  <si>
+    <t>Quitter une équipe de laquelle ont ne fait pas partie</t>
+  </si>
+  <si>
+    <t>Modifier les données d'une de mes équipe</t>
+  </si>
+  <si>
+    <t>Affichage des données de l'équipe, de sa note, de ses membres et de ses projets</t>
+  </si>
+  <si>
+    <t>Enregistrement des modifications</t>
+  </si>
+  <si>
+    <t>Utilisateur</t>
+  </si>
+  <si>
+    <t>Affichage des données de l'utilisateur, de ses équipes et de ses projets</t>
+  </si>
+  <si>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Idem à Ended</t>
+  </si>
+  <si>
+    <t>Affichage des données du projet, de l'équipe mandante et des ressources + possibilité d'apply</t>
+  </si>
+  <si>
+    <t>Proposal - Arrivée sur la page d'un projet en lien</t>
+  </si>
+  <si>
+    <t>Ongoing - Arrivée sur la page d'un projet en lien</t>
+  </si>
+  <si>
+    <t>Idem à Proposal (sans apply) + affichage de l'équipe de développeurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idem à Proposal (sans apply) + affichage de la note et du feedback </t>
+  </si>
+  <si>
+    <t>Idem à Proposal + ajout de ressources + (owner) possibilité de voir les devis et de choisir une candidature</t>
+  </si>
+  <si>
+    <t>Idem à Proposal + ajout de ressources + (owner) possibilité d'ajouter un feedback et une note (cloture)</t>
+  </si>
+  <si>
+    <t>Projet - Proposal</t>
+  </si>
+  <si>
+    <t>Apply avec une équipe</t>
+  </si>
+  <si>
+    <t>Projet - Ongoing</t>
+  </si>
+  <si>
+    <t>Projet - Ended</t>
+  </si>
+  <si>
+    <t>Projet - Abandoned</t>
+  </si>
+  <si>
+    <t>Arrivée sur la page sans lien avec ce projet</t>
+  </si>
+  <si>
+    <t>Demande de prix et d'un document de spécifications, validation par l'upload du document</t>
+  </si>
+  <si>
+    <t>Acceptation d'une équipe candidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet </t>
+  </si>
+  <si>
+    <t>Ajout d'une ressource</t>
+  </si>
+  <si>
+    <t>Ajout du fichier dans la liste des ressources + notification</t>
+  </si>
+  <si>
+    <t>Assignation d'une note et d'un feedback</t>
+  </si>
+  <si>
+    <t>Changement du statut du projet en Ongoing + notification</t>
+  </si>
+  <si>
+    <t>Modifier les données d'un de mes projets</t>
+  </si>
+  <si>
+    <t>Changement du statut du projet en Ended + notification + recalcul de la note globale de l'équipe dev.</t>
+  </si>
+  <si>
+    <t>Création d'un projet avec une deadline dans le passé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,15 +349,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,11 +366,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -300,12 +420,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -335,10 +454,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -652,18 +769,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" customWidth="1"/>
+    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -761,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>1</v>
@@ -786,10 +903,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>1</v>
@@ -800,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>12</v>
@@ -814,10 +931,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>1</v>
@@ -828,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>12</v>
@@ -839,13 +956,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>1</v>
@@ -853,13 +970,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>1</v>
@@ -867,13 +984,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>1</v>
@@ -881,432 +998,634 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="B32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D32" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D33" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D34" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
-      <c r="K60" s="6"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="K65" s="6"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="8"/>
+      <c r="C76" s="6"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="8"/>
+      <c r="C77" s="6"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" s="7" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="12"/>
-    </row>
-    <row r="81" spans="1:11" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="16"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
@@ -1315,16 +1634,10 @@
       <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="9"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="11"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="8"/>
-      <c r="E83" s="10"/>
-      <c r="G83" s="10"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
@@ -1332,6 +1645,40 @@
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
+    <row r="85" spans="1:11" s="7" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="5"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="12"/>
+    </row>
+    <row r="86" spans="1:11" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="15"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="16"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="9"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>